<commit_message>
Actually handling all cell values as strings; cleaning up.
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Heading 1</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Formula</t>
+  </si>
+  <si>
+    <t>Format</t>
   </si>
 </sst>
 </file>
@@ -436,9 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -450,21 +448,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1001</v>
@@ -479,7 +477,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>1001</v>
@@ -494,7 +492,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>1001</v>
@@ -509,7 +507,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>1001</v>
@@ -524,7 +522,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>1001</v>
@@ -539,7 +537,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1001</v>

</xml_diff>

<commit_message>
Fixed error reading Excel files with blank first column cells.
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\excel\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="15555" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Text</t>
   </si>
@@ -109,6 +114,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -434,19 +447,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -460,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -475,7 +490,7 @@
         <v>2002.01</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -486,11 +501,11 @@
         <v>1001.01</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="0">B3+C3</f>
-        <v>2002.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <f t="shared" ref="D3:D9" si="0">B3+C3</f>
+        <v>2002.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -505,7 +520,7 @@
         <v>2002.01</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -520,7 +535,7 @@
         <v>2002.01</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -535,7 +550,7 @@
         <v>2002.01</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -546,6 +561,33 @@
         <v>1001.01</v>
       </c>
       <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>2002.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1001</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1001.01</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>2002.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1001.01</v>
+      </c>
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>2002.01</v>
       </c>

</xml_diff>